<commit_message>
updated excel w ST and DT
</commit_message>
<xml_diff>
--- a/subject_info.xlsx
+++ b/subject_info.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chose\Box\DHI-Lab\CSTAR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chose\Box\C-STAR Pilot\CSTAR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4BF72D1-11A2-4A04-A210-0D8C0D6E7F5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E61FFC09-22AA-4ED9-BF42-ADC1B8E6E71A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{57EA6345-879C-47C4-BA35-5BEFDD08E520}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="137">
   <si>
     <t>Subject ID</t>
   </si>
@@ -452,6 +452,12 @@
   </si>
   <si>
     <t>DHI</t>
+  </si>
+  <si>
+    <t>tug_st_time</t>
+  </si>
+  <si>
+    <t>tug_dt_time</t>
   </si>
 </sst>
 </file>
@@ -902,6 +908,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -932,7 +939,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1157,9 +1163,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{7830FED7-7667-4CE3-A654-F54EABC6A83C}" name="Table18" displayName="Table18" ref="A1:Q43" totalsRowShown="0">
-  <autoFilter ref="A1:Q43" xr:uid="{7830FED7-7667-4CE3-A654-F54EABC6A83C}"/>
-  <tableColumns count="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{7830FED7-7667-4CE3-A654-F54EABC6A83C}" name="Table18" displayName="Table18" ref="A1:S43" totalsRowShown="0">
+  <autoFilter ref="A1:S43" xr:uid="{7830FED7-7667-4CE3-A654-F54EABC6A83C}"/>
+  <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{C044C6D2-CE0C-4909-9FBB-B96EDCB1FCAC}" name="ID" dataDxfId="36"/>
     <tableColumn id="2" xr3:uid="{34919B2F-5D0B-4C75-B0BA-9FA545CC6BEE}" name="Age" dataDxfId="35"/>
     <tableColumn id="3" xr3:uid="{CBB48687-91A3-4808-A9C3-5F03535C4FB2}" name="Sex" dataDxfId="34"/>
@@ -1179,6 +1185,8 @@
     <tableColumn id="15" xr3:uid="{450A1504-AE23-4973-B2E6-A98413963B73}" name="VOMs"/>
     <tableColumn id="16" xr3:uid="{2296B09E-33DE-4BBD-90A1-C57DCFB35AC3}" name="MiniBEST"/>
     <tableColumn id="17" xr3:uid="{2CEAFE56-C0EB-48F3-83C2-8AE69790CA37}" name="DHI"/>
+    <tableColumn id="18" xr3:uid="{EA4D983C-6A4E-45A4-B49C-7AACE7F80DC3}" name="tug_st_time"/>
+    <tableColumn id="19" xr3:uid="{76B0A8CB-B51A-4D7F-9AC5-82D1ECE722E6}" name="tug_dt_time"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1545,10 +1553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF15B6FB-64A7-487C-83A8-9CFD833F5CA1}">
-  <dimension ref="A1:Q43"/>
+  <dimension ref="A1:S43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q25"/>
+      <selection activeCell="U21" sqref="U21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1556,7 +1564,7 @@
     <col min="4" max="4" width="8.88671875" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>113</v>
       </c>
@@ -1605,11 +1613,17 @@
       <c r="P1" t="s">
         <v>126</v>
       </c>
-      <c r="Q1" s="30" t="s">
+      <c r="Q1" s="20" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R1" t="s">
+        <v>135</v>
+      </c>
+      <c r="S1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>75</v>
       </c>
@@ -1663,7 +1677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>76</v>
       </c>
@@ -1716,8 +1730,14 @@
       <c r="Q3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R3">
+        <v>7</v>
+      </c>
+      <c r="S3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>86</v>
       </c>
@@ -1771,7 +1791,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>80</v>
       </c>
@@ -1824,8 +1844,14 @@
       <c r="Q5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R5">
+        <v>8</v>
+      </c>
+      <c r="S5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>81</v>
       </c>
@@ -1878,8 +1904,14 @@
       <c r="Q6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R6">
+        <v>8</v>
+      </c>
+      <c r="S6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>83</v>
       </c>
@@ -1932,8 +1964,14 @@
       <c r="Q7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R7">
+        <v>9</v>
+      </c>
+      <c r="S7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>89</v>
       </c>
@@ -1986,8 +2024,14 @@
       <c r="Q8">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R8">
+        <v>9</v>
+      </c>
+      <c r="S8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>93</v>
       </c>
@@ -2040,8 +2084,14 @@
       <c r="Q9">
         <v>44</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R9">
+        <v>12</v>
+      </c>
+      <c r="S9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>94</v>
       </c>
@@ -2094,8 +2144,14 @@
       <c r="Q10">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R10">
+        <v>11</v>
+      </c>
+      <c r="S10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>97</v>
       </c>
@@ -2148,8 +2204,14 @@
       <c r="Q11">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R11">
+        <v>11</v>
+      </c>
+      <c r="S11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>99</v>
       </c>
@@ -2202,8 +2264,14 @@
       <c r="Q12">
         <v>32</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R12">
+        <v>12</v>
+      </c>
+      <c r="S12">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>100</v>
       </c>
@@ -2256,8 +2324,14 @@
       <c r="Q13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R13">
+        <v>10</v>
+      </c>
+      <c r="S13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>101</v>
       </c>
@@ -2310,8 +2384,14 @@
       <c r="Q14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R14">
+        <v>9</v>
+      </c>
+      <c r="S14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>102</v>
       </c>
@@ -2364,8 +2444,14 @@
       <c r="Q15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R15">
+        <v>11</v>
+      </c>
+      <c r="S15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>103</v>
       </c>
@@ -2418,8 +2504,14 @@
       <c r="Q16">
         <v>34</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R16">
+        <v>12</v>
+      </c>
+      <c r="S16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>104</v>
       </c>
@@ -2472,8 +2564,14 @@
       <c r="Q17">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R17">
+        <v>14</v>
+      </c>
+      <c r="S17">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>107</v>
       </c>
@@ -2526,8 +2624,14 @@
       <c r="Q18">
         <v>40</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R18">
+        <v>12</v>
+      </c>
+      <c r="S18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>109</v>
       </c>
@@ -2580,8 +2684,14 @@
       <c r="Q19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R19">
+        <v>10</v>
+      </c>
+      <c r="S19">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>110</v>
       </c>
@@ -2634,8 +2744,14 @@
       <c r="Q20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R20">
+        <v>10</v>
+      </c>
+      <c r="S20">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>111</v>
       </c>
@@ -2688,8 +2804,14 @@
       <c r="Q21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R21">
+        <v>8</v>
+      </c>
+      <c r="S21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>112</v>
       </c>
@@ -2742,8 +2864,14 @@
       <c r="Q22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R22">
+        <v>9</v>
+      </c>
+      <c r="S22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>127</v>
       </c>
@@ -2796,8 +2924,14 @@
       <c r="Q23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R23">
+        <v>9</v>
+      </c>
+      <c r="S23">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>128</v>
       </c>
@@ -2850,8 +2984,14 @@
       <c r="Q24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R24">
+        <v>10</v>
+      </c>
+      <c r="S24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>5</v>
       </c>
@@ -2871,7 +3011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>6</v>
       </c>
@@ -2891,7 +3031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>7</v>
       </c>
@@ -2911,7 +3051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>8</v>
       </c>
@@ -2931,7 +3071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>9</v>
       </c>
@@ -2951,7 +3091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>10</v>
       </c>
@@ -2971,7 +3111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>11</v>
       </c>
@@ -2991,7 +3131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>12</v>
       </c>
@@ -6522,31 +6662,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="22"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="22"/>
+      <c r="A1" s="23"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="23"/>
     </row>
     <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="24" t="s">
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="22"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="23"/>
     </row>
     <row r="3" spans="1:8" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
       <c r="D3" s="11">
         <v>1</v>
       </c>
@@ -6559,11 +6699,11 @@
       <c r="G3" s="13">
         <v>4</v>
       </c>
-      <c r="H3" s="22"/>
+      <c r="H3" s="23"/>
     </row>
     <row r="4" spans="1:8" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="23"/>
-      <c r="B4" s="27" t="s">
+      <c r="A4" s="24"/>
+      <c r="B4" s="28" t="s">
         <v>37</v>
       </c>
       <c r="C4" s="14" t="s">
@@ -6581,11 +6721,11 @@
       <c r="G4" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H4" s="22"/>
+      <c r="H4" s="23"/>
     </row>
     <row r="5" spans="1:8" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="23"/>
-      <c r="B5" s="28"/>
+      <c r="A5" s="24"/>
+      <c r="B5" s="29"/>
       <c r="C5" s="15" t="s">
         <v>64</v>
       </c>
@@ -6601,11 +6741,11 @@
       <c r="G5" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="H5" s="22"/>
+      <c r="H5" s="23"/>
     </row>
     <row r="6" spans="1:8" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="23"/>
-      <c r="B6" s="28"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="29"/>
       <c r="C6" s="15" t="s">
         <v>63</v>
       </c>
@@ -6621,11 +6761,11 @@
       <c r="G6" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="H6" s="22"/>
+      <c r="H6" s="23"/>
     </row>
     <row r="7" spans="1:8" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="23"/>
-      <c r="B7" s="28"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="29"/>
       <c r="C7" s="16" t="s">
         <v>60</v>
       </c>
@@ -6641,11 +6781,11 @@
       <c r="G7" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="H7" s="22"/>
+      <c r="H7" s="23"/>
     </row>
     <row r="8" spans="1:8" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="23"/>
-      <c r="B8" s="28"/>
+      <c r="A8" s="24"/>
+      <c r="B8" s="29"/>
       <c r="C8" s="16" t="s">
         <v>62</v>
       </c>
@@ -6661,11 +6801,11 @@
       <c r="G8" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="H8" s="22"/>
+      <c r="H8" s="23"/>
     </row>
     <row r="9" spans="1:8" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="23"/>
-      <c r="B9" s="29"/>
+      <c r="A9" s="24"/>
+      <c r="B9" s="30"/>
       <c r="C9" s="17" t="s">
         <v>59</v>
       </c>
@@ -6681,16 +6821,16 @@
       <c r="G9" s="10">
         <v>5</v>
       </c>
-      <c r="H9" s="22"/>
+      <c r="H9" s="23"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="22"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
change from dhi to S##
</commit_message>
<xml_diff>
--- a/subject_info.xlsx
+++ b/subject_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chose\Box\C-STAR Pilot\CSTAR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E61FFC09-22AA-4ED9-BF42-ADC1B8E6E71A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7CC644-2BBC-4E69-84E6-A33A3AD65946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{57EA6345-879C-47C4-BA35-5BEFDD08E520}"/>
+    <workbookView xWindow="-75" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{57EA6345-879C-47C4-BA35-5BEFDD08E520}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="7" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="138">
   <si>
     <t>Subject ID</t>
   </si>
@@ -458,6 +458,9 @@
   </si>
   <si>
     <t>tug_dt_time</t>
+  </si>
+  <si>
+    <t>S30</t>
   </si>
 </sst>
 </file>
@@ -1553,10 +1556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF15B6FB-64A7-487C-83A8-9CFD833F5CA1}">
-  <dimension ref="A1:S43"/>
+  <dimension ref="A1:V43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U21" sqref="U21"/>
+      <selection activeCell="V25" sqref="V25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1564,7 +1567,7 @@
     <col min="4" max="4" width="8.88671875" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>113</v>
       </c>
@@ -1623,9 +1626,9 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B2" s="18">
         <v>19</v>
@@ -1677,9 +1680,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B3" s="18">
         <v>44</v>
@@ -1737,7 +1740,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>86</v>
       </c>
@@ -1790,10 +1793,12 @@
       <c r="Q4">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B5" s="18">
         <v>50</v>
@@ -1850,10 +1855,12 @@
       <c r="S5">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B6" s="18">
         <v>42</v>
@@ -1910,10 +1917,12 @@
       <c r="S6">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B7" s="18">
         <v>32</v>
@@ -1970,8 +1979,10 @@
       <c r="S7">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>89</v>
       </c>
@@ -2030,8 +2041,10 @@
       <c r="S8">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>93</v>
       </c>
@@ -2090,8 +2103,10 @@
       <c r="S9">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>94</v>
       </c>
@@ -2150,8 +2165,10 @@
       <c r="S10">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>97</v>
       </c>
@@ -2210,8 +2227,10 @@
       <c r="S11">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>99</v>
       </c>
@@ -2270,8 +2289,10 @@
       <c r="S12">
         <v>11.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>100</v>
       </c>
@@ -2330,10 +2351,12 @@
       <c r="S13">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="B14" s="18">
         <v>28</v>
@@ -2390,10 +2413,12 @@
       <c r="S14">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="B15" s="18">
         <v>42</v>
@@ -2450,8 +2475,10 @@
       <c r="S15">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>103</v>
       </c>
@@ -2510,8 +2537,10 @@
       <c r="S16">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>104</v>
       </c>
@@ -2570,8 +2599,10 @@
       <c r="S17">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>107</v>
       </c>
@@ -2630,10 +2661,12 @@
       <c r="S18">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="B19" s="18">
         <v>26</v>
@@ -2690,10 +2723,12 @@
       <c r="S19">
         <v>13</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="B20" s="18">
         <v>32</v>
@@ -2750,10 +2785,12 @@
       <c r="S20">
         <v>12</v>
       </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="B21" s="18">
         <v>22</v>
@@ -2810,10 +2847,12 @@
       <c r="S21">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>112</v>
+        <v>137</v>
       </c>
       <c r="B22" s="18">
         <v>25</v>
@@ -2870,8 +2909,10 @@
       <c r="S22">
         <v>10</v>
       </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>127</v>
       </c>
@@ -2930,8 +2971,10 @@
       <c r="S23">
         <v>12</v>
       </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>128</v>
       </c>
@@ -2990,8 +3033,10 @@
       <c r="S24">
         <v>10</v>
       </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>5</v>
       </c>
@@ -3011,7 +3056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>6</v>
       </c>
@@ -3031,7 +3076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>7</v>
       </c>
@@ -3051,7 +3096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>8</v>
       </c>
@@ -3071,7 +3116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>9</v>
       </c>
@@ -3091,7 +3136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>10</v>
       </c>
@@ -3111,7 +3156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>11</v>
       </c>
@@ -3131,7 +3176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>12</v>
       </c>
@@ -3393,8 +3438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DC1054C-FE9B-49DE-AC90-AF26B54F8E5A}">
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4164,7 +4209,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:F20"/>
+      <selection pane="bottomLeft" activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>